<commit_message>
Update to Excel spreadsheet - added notes based on call with Mia on 1/14/20
</commit_message>
<xml_diff>
--- a/list_of_abx_org_and_order_names_in_cs_data.xlsx
+++ b/list_of_abx_org_and_order_names_in_cs_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreynolds2/Documents/GitHub/MS-Antibiogram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131AC08B-F619-E844-B52A-CE7F074C65ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FBCAB2-889B-0B40-B75A-C897224F5D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="500" windowWidth="23140" windowHeight="17960" activeTab="2" xr2:uid="{A81D0479-BAD1-CE48-9386-97F13F9E1195}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23680" windowHeight="20600" activeTab="2" xr2:uid="{A81D0479-BAD1-CE48-9386-97F13F9E1195}"/>
   </bookViews>
   <sheets>
     <sheet name="abx" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="374">
   <si>
     <t>Amikacin</t>
   </si>
@@ -1165,12 +1165,30 @@
   <si>
     <t>For our data, there is Staph aur (+ methicillin resistance, vancomycin resistant, and nafcillin resistant).</t>
   </si>
+  <si>
+    <t>1. Is there a threshold to determining what ABX should be included on the antibiogram?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Those that align with good ABX stewardship. </t>
+  </si>
+  <si>
+    <t>Central- Big, stable IVs.</t>
+  </si>
+  <si>
+    <t>Take bacterial culture from IV itself.</t>
+  </si>
+  <si>
+    <t>MRSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSSA *Methicillin sensitive </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1212,6 +1230,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1239,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1268,6 +1293,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1582,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4DBF902-B672-704E-80D5-0AB4920022A7}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1604,16 +1630,16 @@
     <col min="34" max="34" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>32</v>
@@ -1622,8 +1648,11 @@
         <v>33</v>
       </c>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1634,8 +1663,11 @@
         <v>9605</v>
       </c>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1646,8 +1678,11 @@
         <v>8644</v>
       </c>
       <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -1659,7 +1694,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -1671,7 +1706,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1683,7 +1718,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -1695,7 +1730,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -1707,7 +1742,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -1719,7 +1754,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -1731,7 +1766,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -1743,7 +1778,7 @@
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -1755,7 +1790,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -1767,7 +1802,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2501,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8491D5-A7C0-8845-8983-27A57119E164}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B20"/>
+    <sheetView topLeftCell="A6" zoomScale="116" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2514,15 +2549,15 @@
     <col min="3" max="3" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>52</v>
@@ -2531,7 +2566,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -2542,7 +2577,7 @@
         <v>60348</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2553,7 +2588,7 @@
         <v>37366</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -2564,7 +2599,7 @@
         <v>17448</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>4</v>
       </c>
@@ -2575,7 +2610,7 @@
         <v>16743</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -2586,7 +2621,7 @@
         <v>14985</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>6</v>
       </c>
@@ -2597,7 +2632,7 @@
         <v>5954</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7</v>
       </c>
@@ -2608,7 +2643,7 @@
         <v>5302</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>8</v>
       </c>
@@ -2618,8 +2653,11 @@
       <c r="C11" s="10">
         <v>3623</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>9</v>
       </c>
@@ -2629,8 +2667,11 @@
       <c r="C12" s="10">
         <v>2512</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>10</v>
       </c>
@@ -2641,7 +2682,7 @@
         <v>1938</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>11</v>
       </c>
@@ -2652,7 +2693,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>12</v>
       </c>
@@ -2663,7 +2704,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>13</v>
       </c>
@@ -2884,7 +2925,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="14" t="s">
         <v>357</v>
       </c>
     </row>
@@ -2912,8 +2953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6C18CF-A363-294F-BF04-E0CC0C211D0F}">
   <dimension ref="A1:E221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B48" sqref="B23:C48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3002,6 +3043,9 @@
       <c r="C8" s="10">
         <v>12785</v>
       </c>
+      <c r="D8" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -3057,6 +3101,9 @@
       </c>
       <c r="C13" s="10">
         <v>6366</v>
+      </c>
+      <c r="D13" t="s">
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>